<commit_message>
Update alk class tests
</commit_message>
<xml_diff>
--- a/manually_collected_data/inputs/Apocynaceae traits.xlsx
+++ b/manually_collected_data/inputs/Apocynaceae traits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25915"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26018"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rbgkew-my.sharepoint.com/personal/c_aitken_kew_org/Documents/3M Project/Apocynaceae/Literature Review - Trait Data/Literature review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B8DF125-D716-4537-96A1-CB718D2CF1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{77D093DE-4113-45DF-BB43-13D2369B0E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="615" windowWidth="20850" windowHeight="23385" firstSheet="2" xr2:uid="{86832E41-84C4-4AB2-BAFD-DA8ED13F0409}"/>
+    <workbookView xWindow="3120" yWindow="615" windowWidth="20850" windowHeight="23385" xr2:uid="{86832E41-84C4-4AB2-BAFD-DA8ED13F0409}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3170" uniqueCount="1511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3157" uniqueCount="1511">
   <si>
     <t>Genus</t>
   </si>
@@ -20343,7 +20343,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -20631,7 +20631,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -20642,8 +20642,8 @@
   <dimension ref="A1:K933"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="A2:K781"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C738" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="C744" sqref="C744:E744"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
     </sheetView>
@@ -20773,12 +20773,7 @@
       <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="4">
-        <v>143</v>
-      </c>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
@@ -21653,12 +21648,7 @@
       <c r="B58" t="s">
         <v>98</v>
       </c>
-      <c r="C58" t="s">
-        <v>13</v>
-      </c>
-      <c r="E58" s="4">
-        <v>143</v>
-      </c>
+      <c r="E58" s="4"/>
     </row>
     <row r="59" spans="1:11">
       <c r="A59" t="s">
@@ -21667,12 +21657,7 @@
       <c r="B59" t="s">
         <v>100</v>
       </c>
-      <c r="C59" t="s">
-        <v>13</v>
-      </c>
-      <c r="E59" s="4">
-        <v>143</v>
-      </c>
+      <c r="E59" s="4"/>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" t="s">
@@ -24524,12 +24509,7 @@
       <c r="B234" t="s">
         <v>376</v>
       </c>
-      <c r="C234" t="s">
-        <v>13</v>
-      </c>
-      <c r="E234" s="4">
-        <v>143</v>
-      </c>
+      <c r="E234" s="4"/>
     </row>
     <row r="235" spans="1:11">
       <c r="A235" t="s">
@@ -24579,12 +24559,7 @@
       <c r="B242" t="s">
         <v>385</v>
       </c>
-      <c r="C242" t="s">
-        <v>13</v>
-      </c>
-      <c r="E242" s="4">
-        <v>143</v>
-      </c>
+      <c r="E242" s="4"/>
     </row>
     <row r="243" spans="1:11">
       <c r="A243" t="s">
@@ -26292,12 +26267,7 @@
       <c r="B352" t="s">
         <v>560</v>
       </c>
-      <c r="C352" t="s">
-        <v>13</v>
-      </c>
-      <c r="E352" s="4">
-        <v>143</v>
-      </c>
+      <c r="E352" s="4"/>
     </row>
     <row r="353" spans="1:11">
       <c r="A353" t="s">
@@ -26650,13 +26620,8 @@
       <c r="B379" t="s">
         <v>597</v>
       </c>
-      <c r="C379" t="s">
-        <v>13</v>
-      </c>
       <c r="D379"/>
-      <c r="E379" s="4">
-        <v>143</v>
-      </c>
+      <c r="E379" s="4"/>
     </row>
     <row r="380" spans="1:5">
       <c r="A380" t="s">
@@ -26952,12 +26917,7 @@
       <c r="B403" t="s">
         <v>627</v>
       </c>
-      <c r="C403" t="s">
-        <v>13</v>
-      </c>
-      <c r="E403" s="4">
-        <v>143</v>
-      </c>
+      <c r="E403" s="4"/>
     </row>
     <row r="404" spans="1:5">
       <c r="A404" t="s">
@@ -27412,12 +27372,7 @@
       <c r="B439" t="s">
         <v>675</v>
       </c>
-      <c r="C439" t="s">
-        <v>13</v>
-      </c>
-      <c r="E439" s="4">
-        <v>143</v>
-      </c>
+      <c r="E439" s="4"/>
     </row>
     <row r="440" spans="1:11">
       <c r="A440" t="s">
@@ -28026,12 +27981,7 @@
       <c r="B486" t="s">
         <v>742</v>
       </c>
-      <c r="C486" t="s">
-        <v>13</v>
-      </c>
-      <c r="E486" s="4">
-        <v>143</v>
-      </c>
+      <c r="E486" s="4"/>
     </row>
     <row r="487" spans="1:11">
       <c r="A487" t="s">
@@ -31275,12 +31225,7 @@
       <c r="B722" t="s">
         <v>1048</v>
       </c>
-      <c r="C722" t="s">
-        <v>13</v>
-      </c>
-      <c r="E722" s="4">
-        <v>143</v>
-      </c>
+      <c r="E722" s="4"/>
     </row>
     <row r="723" spans="1:11">
       <c r="A723" t="s">
@@ -31306,12 +31251,7 @@
       <c r="B724" t="s">
         <v>1050</v>
       </c>
-      <c r="C724" t="s">
-        <v>13</v>
-      </c>
-      <c r="E724" s="4">
-        <v>143</v>
-      </c>
+      <c r="E724" s="4"/>
     </row>
     <row r="725" spans="1:11">
       <c r="A725" t="s">
@@ -31609,12 +31549,7 @@
       <c r="B744" t="s">
         <v>1078</v>
       </c>
-      <c r="C744" t="s">
-        <v>13</v>
-      </c>
-      <c r="E744" s="4">
-        <v>143</v>
-      </c>
+      <c r="E744" s="4"/>
     </row>
     <row r="745" spans="1:7">
       <c r="A745" t="s">

</xml_diff>